<commit_message>
Add commit date: Mon Sep 23 13:03:09 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SQL" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Python" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Links" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bash" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SQL" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Python" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Links" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Bash" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,6 +621,26 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>Вывод всех записей таблицы</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1162</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Тестовое сообщение</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Тестовое сообщение</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Тестовое сообщение</t>
         </is>
       </c>
     </row>
@@ -635,7 +655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1136,6 +1156,26 @@
       <c r="D29" t="inlineStr">
         <is>
           <t>Метод загружает csv файл с данными.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2090</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Тестовое сообщение</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Тестовое сообщение</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Тестовое сообщение1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add commit date: Thu Sep 26 17:55:43 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -430,7 +430,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>INSERT INTO  git_and_bash (command, name) VALUES ('test', 'test')</t>
+          <t>INSERT INTO git_and_bash (command, name) VALUES ('test', 'test')</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT * FROM git_and_bash WHERE command LIKE '%ls%' </t>
+          <t>SELECT * FROM git_and_bash WHERE command LIKE '%ls%'</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SELECT DISTINCT field_299 FROM app_entity_25;</t>
+          <t>SELECT DISTINCT field FROM table;</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT * FROM app_entity_30 </t>
+          <t>SELECT * FROM table;</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Подсчёт количества строк в датафрейме.</t>
+          <t>Подсчёт количества строк в датафрейме</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Вывод статистических сведений о датафрейме.</t>
+          <t>Вывод статистических сведений о датафрейме</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -790,7 +790,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Для того чтобы подсчитать количество значений в конкретном столбце, можно воспользоваться следующей конструкцие.</t>
+          <t>Для того чтобы подсчитать количество значений в конкретном столбце, можно воспользоваться следующей конструкцие</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Получение списка значений столбцов.</t>
+          <t>Получение списка значений столбцов</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">df = pd.read_excel('sotr.xlsx', index_col=0)  </t>
+          <t>df = pd.read_excel('sotr.xlsx', index_col=0)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD  с описанием и примерами</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1380,8 +1380,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Как создать и запустить bat-файлы
-</t>
+          <t>Как создать и запустить bat-файлы</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1418,7 +1417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,12 +1436,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Удаление последней набранной строки.</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Комбинация удаляет последнюю набранную пользователем команду.</t>
+          <t>Удаление последней набранной строки</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1454,6 @@
           <t>Поиск текста в истории</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1476,11 +1469,6 @@
           <t>Копирование файлов</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Данная команда копирует файл bash_and_git.txt в папку корня draft-project.</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1496,11 +1484,6 @@
           <t>Очистка экрана</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Команда очищает экран.</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1513,12 +1496,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Завершает процесс.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Команда завершает определенный запущенный процесс.</t>
+          <t>Завершает процесс</t>
         </is>
       </c>
     </row>
@@ -1533,12 +1511,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>История команд.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Команда выводить всю историю команд bash.</t>
+          <t>История команд</t>
         </is>
       </c>
     </row>
@@ -1556,11 +1529,6 @@
           <t>Выводит список процессов</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Выводит весь список запущенных процессов.</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1576,11 +1544,6 @@
           <t>Показывает текущий путь к папке</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Показывает текущий путь к папке</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1596,11 +1559,6 @@
           <t>Возврат в вышестоящую директорию</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Команда возвращает на каталог выше.</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1616,11 +1574,6 @@
           <t>Возврат на две папки выше</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Команда возвращает на 2 каталога выше.</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1633,12 +1586,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Переход в корневую папку.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Команда делает переход в корневую папку, в windows это папка пользователя системы.</t>
+          <t>Переход в корневую папку</t>
         </is>
       </c>
     </row>
@@ -1656,11 +1604,6 @@
           <t>Вывод содержимого каталога(файлов и папок)</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Вывод содержимого каталога(файлов и папок)</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1676,11 +1619,6 @@
           <t>Вернуться назад</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Команда возвращает в выше стоящюю директорию.</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1696,7 +1634,6 @@
           <t>Переход  в оперделенную папку</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1712,7 +1649,6 @@
           <t>Показать файлы в данной папке, включая и скрытые</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1728,7 +1664,6 @@
           <t>Вывод папок раздела</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1744,7 +1679,6 @@
           <t>Создание папки или папок(несколько папок через пробел нужно указать)</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1760,7 +1694,6 @@
           <t>Файл intro перенесется в папку manual под именем chap1</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1776,7 +1709,6 @@
           <t>Файл chap3 перенесется в папку manual</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1792,7 +1724,6 @@
           <t>Файл appendix переименуется в apndx.a</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1808,7 +1739,6 @@
           <t>Чтение указанного файла</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1824,7 +1754,6 @@
           <t>Удаление файла</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1840,7 +1769,6 @@
           <t>Удаление папки с содержанием</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1856,7 +1784,6 @@
           <t>Удаление папки с содержанием принудительно</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1872,7 +1799,6 @@
           <t>Выход из командной строки</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1888,7 +1814,6 @@
           <t>Запрос DNS определенного адреса</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1904,7 +1829,6 @@
           <t>Запуск процесса в фоновом режиме</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1920,7 +1844,6 @@
           <t>Генерация ssh-ключа</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1936,7 +1859,6 @@
           <t>Создание виртуального окружения Python</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1952,7 +1874,6 @@
           <t>Создание файла скрипта bash.sh</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1968,7 +1889,6 @@
           <t>Открытие файла встроенным bash редактором</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1984,7 +1904,6 @@
           <t>Запуск скрипта bash</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2000,7 +1919,6 @@
           <t>Настройка прав на файл скрипта</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2016,7 +1934,6 @@
           <t>Выводит списокм папки и файлы текущего раздела с датой изменения, размером и правами доступа</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2032,11 +1949,6 @@
           <t>Удаляет все файлы в текущей директории</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2052,7 +1964,6 @@
           <t>Удаляет все команды из истории</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2068,7 +1979,6 @@
           <t>Вывод текущей даты и времени</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2084,7 +1994,6 @@
           <t>Создаем две папки в текущем каталоге</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2100,7 +2009,6 @@
           <t>Удаление всех папок текущей директории</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2116,7 +2024,6 @@
           <t>Установки нужной библиотеки</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2129,10 +2036,9 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Переход из текущего раздела в другой раздел с определенной папкой.</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
+          <t>Переход из текущего раздела в другой раздел с определенной папкой</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2145,10 +2051,9 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Выводит на экран все файлы с указанным расширением.</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr"/>
+          <t>Выводит на экран все файлы с указанным расширением</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2161,12 +2066,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Вернуться в корневую папку.</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Команда возвращает пользователя в корневую папку.</t>
+          <t>Вернуться в корневую папку</t>
         </is>
       </c>
     </row>
@@ -2184,11 +2084,6 @@
           <t>Копирование всех файлов в другую папку</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Указанная команда скопирует все файлы одной папки в другую папку.</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2204,11 +2099,6 @@
           <t>Поиск процесса по имени</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Команда позволяет в данном случае найти все процессы с именем python</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2224,11 +2114,6 @@
           <t>Завершить работы всех приложений python</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Завершить работы всех приложений python</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2244,11 +2129,6 @@
           <t>Вывод всех процессов Windows по имени</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Команда PowerShell, которая выводит все процессы Windows с названием python.</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2264,11 +2144,6 @@
           <t>Остановка процессов по имени</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Команда PowerShell, которая останавливает все процессы Windows с названием python, аналог команды kill в Bash.</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2284,11 +2159,6 @@
           <t>Удаление папки с файлами в PowerShell</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Команда удаляет папку с файлами в PowerSHell</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2304,11 +2174,6 @@
           <t>Создание файла с пакетами</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Команда создает файл с пакетами. </t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2324,11 +2189,6 @@
           <t>Устанавливает из файла все пакеты</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Устанавливает из файла все пакеты.</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2344,11 +2204,6 @@
           <t>Перемещение файла из текущей папки в вышестоящий раздел</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Перемещение файла из текущей папки в вышестоящий раздел</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2364,11 +2219,6 @@
           <t>Перемещение нескольких файлов в другую папку с определенным расширением</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Перемещение нескольких файлов в другую папку с определенным расширением</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2384,11 +2234,6 @@
           <t>Запуск bash скрипта из любой директории</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Запуск bash скрипта из любой директории, указывается полный путь к исполняемому файлу.</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2404,7 +2249,6 @@
           <t>Назначение git глобальной почты</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2420,7 +2264,6 @@
           <t>Назначение git глобального имени</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2433,12 +2276,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Клонирование удаленного репозитория.</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Команда клонирует с удаленного репозитория проект.</t>
+          <t>Клонирование удаленного репозитория</t>
         </is>
       </c>
     </row>
@@ -2453,12 +2291,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Статус изменений.</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Команда выводит статус всех изменений на данный момент.</t>
+          <t>Статус изменений</t>
         </is>
       </c>
     </row>
@@ -2476,7 +2309,6 @@
           <t>Вывод конфигурации git</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2489,12 +2321,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Подготовка файлов для коммита.</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Данная команда фиксирует все текущие изменения всех файлов, кроме тех, которые указаны в gitignore.</t>
+          <t>Подготовка файлов для коммита</t>
         </is>
       </c>
     </row>
@@ -2509,12 +2336,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Подготовка коммита.</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Команда создает коммит с указанием комментария.</t>
+          <t>Подготовка коммита</t>
         </is>
       </c>
     </row>
@@ -2532,11 +2354,6 @@
           <t>Отправка изменений на репозиторий</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Команда отправляет на сервер репозитория коммит.</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2552,11 +2369,6 @@
           <t>Инициализация git в папке</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Команда инициализирует текущую папку как репозиторий.</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2572,9 +2384,49 @@
           <t>Скачивание изменения из репозитория на локальную машину</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Команда скачивает с репозитория последние измнения.</t>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>92</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>~/AppData/Local/Programs/Python/Python39/python.exe -m pip install --upgrade pip</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Обновление pip</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>93</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>~/AppData/Local/Programs/Python/Python39/python.exe venv/Scripts/pip.exe install pandas</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Установка библиотеки Pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>96</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ТестТестТестТест</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ТестТестТестТест</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add commit date: Tue Oct  1 17:48:25 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -1417,7 +1417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2417,29 +2417,14 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>ТестТестТестТест</t>
+          <t>fsdfffffffffffffffff</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
-        <is>
-          <t>ТестТестТестТест</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>97</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>fsdfffffffffffffffff</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
         <is>
           <t>fsdfffffffffffffffff</t>
         </is>

</xml_diff>

<commit_message>
Add commit date: Wed Oct  2 17:28:59 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -1190,7 +1190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1200,211 +1200,231 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Lorem Ipsum - это текст-"рыба", часто используемый в печати и вэб-дизайне. Lorem Ipsum является стандартной "рыбой" для текстов на латинице с начала XVI века. В то время некий безымянный печатник создал большую коллекцию размеров и форм шрифтов, используя Lorem Ipsum для распечатки образцов. Lorem Ipsum не только успешно пережил без заметных изменений пять веков, но и перешагнул в электронный дизайн. Его популяризации в новое время послужили публикация листов Letraset с образцами Lorem Ipsum в 60-х годах и, в более недавнее время, программы электронной вёрстки типа Aldus PageMaker, в шаблонах которых используется Lorem Ipsum.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
+          <t>Lorem Ipsum - это текст-"рыба", часто используемый в печати и вэб-дизайне. Lorem Ipsum является стандартной "рыбой" для текстов на латинице с начала XVI века. В то время некий безымянный печатник создал большую коллекцию размеров и форм шрифтов, используя Lorem Ipsum для распечатки образцов. Lorem Ipsum не только успешно пережил без заметных изменений пять веков, но и перешагнул в электронный дизайн. Его популяризации в новое время послужили публикация листов Letraset с образцами Lorem Ipsum в 60-х годах и, в более недавнее время, программы электронной вёрстки типа Aldus PageMaker, в шаблонах которых используется Lorem Ipsum.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Lorem Ipsum - это текст-"рыба", часто используемый в печати и вэб-дизайне. Lorem Ipsum является стандартной "рыбой" для текстов на латинице с начала XVI века. В то время некий безымянный печатник создал большую коллекцию размеров и форм шрифтов, используя Lorem Ipsum для распечатки образцов. Lorem Ipsum не только успешно пережил без заметных изменений пять веков, но и перешагнул в электронный дизайн. Его популяризации в новое время послужили публикация листов Letraset с образцами Lorem Ipsum в 60-х годах и, в более недавнее время, программы электронной вёрстки типа Aldus PageMaker, в шаблонах которых используется Lorem Ipsum.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://pypi.org/project/PyMySQL/</t>
+          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://getbootstrap.com/</t>
+          <t>https://pypi.org/project/PyMySQL/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://developer.mozilla.org/ru/docs/Web</t>
+          <t>https://getbootstrap.com/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
+          <t>Документация по Bootstrap.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Работа с gitignore</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>https://developer.mozilla.org/ru/docs/Web</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Сайт с документацией по веб-технологиям.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Работа с gitignore</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://sky.pro/media/pep8/</t>
+          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>https://sky.pro/media/pep8/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://ab57.ru/cmdlist.html</t>
+          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>https://ab57.ru/cmdlist.html</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Как создать и запустить bat-файлы</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>1</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Как сделать скрипт на bash</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add commit date: Thu Oct  3 16:24:33 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,6 +641,46 @@
       <c r="D13" t="inlineStr">
         <is>
           <t>Тестовое сообщение</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1163</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1164</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
         </is>
       </c>
     </row>
@@ -655,7 +695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1176,6 +1216,46 @@
       <c r="D30" t="inlineStr">
         <is>
           <t>Тестовое сообщение1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2091</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TestTestTestTestTestTestTest</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2092</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>пвавапавпав</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>павпвапавпвап</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>вапввввввввв</t>
         </is>
       </c>
     </row>
@@ -1200,21 +1280,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Lorem Ipsum - это текст-"рыба", часто используемый в печати и вэб-дизайне. Lorem Ipsum является стандартной "рыбой" для текстов на латинице с начала XVI века. В то время некий безымянный печатник создал большую коллекцию размеров и форм шрифтов, используя Lorem Ipsum для распечатки образцов. Lorem Ipsum не только успешно пережил без заметных изменений пять веков, но и перешагнул в электронный дизайн. Его популяризации в новое время послужили публикация листов Letraset с образцами Lorem Ipsum в 60-х годах и, в более недавнее время, программы электронной вёрстки типа Aldus PageMaker, в шаблонах которых используется Lorem Ipsum.</t>
+          <t>TestTestTestTestTestTestTest</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Lorem Ipsum - это текст-"рыба", часто используемый в печати и вэб-дизайне. Lorem Ipsum является стандартной "рыбой" для текстов на латинице с начала XVI века. В то время некий безымянный печатник создал большую коллекцию размеров и форм шрифтов, используя Lorem Ipsum для распечатки образцов. Lorem Ipsum не только успешно пережил без заметных изменений пять веков, но и перешагнул в электронный дизайн. Его популяризации в новое время послужили публикация листов Letraset с образцами Lorem Ipsum в 60-х годах и, в более недавнее время, программы электронной вёрстки типа Aldus PageMaker, в шаблонах которых используется Lorem Ipsum.</t>
+          <t>TestTestTestTestTestTestTest</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Lorem Ipsum - это текст-"рыба", часто используемый в печати и вэб-дизайне. Lorem Ipsum является стандартной "рыбой" для текстов на латинице с начала XVI века. В то время некий безымянный печатник создал большую коллекцию размеров и форм шрифтов, используя Lorem Ipsum для распечатки образцов. Lorem Ipsum не только успешно пережил без заметных изменений пять веков, но и перешагнул в электронный дизайн. Его популяризации в новое время послужили публикация листов Letraset с образцами Lorem Ipsum в 60-х годах и, в более недавнее время, программы электронной вёрстки типа Aldus PageMaker, в шаблонах которых используется Lorem Ipsum.</t>
+          <t>TestTestTestTestTestTestTest</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add commit date: Thu Oct  3 16:29:13 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -670,17 +670,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTest</t>
+          <t>TestTestTestTestTestTestTestadasd</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTest</t>
+          <t>TestTestTestTestTestTestTestsadasd</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTest</t>
+          <t>TestTestTestTestTestTestTestasdsad</t>
         </is>
       </c>
     </row>
@@ -1245,17 +1245,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>пвавапавпав</t>
+          <t>пвавапавпавasdasd</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>павпвапавпвап</t>
+          <t>павпвапавпвапasdasd</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>вапввввввввв</t>
+          <t>вапвввввввввasdad</t>
         </is>
       </c>
     </row>
@@ -1284,17 +1284,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTest</t>
+          <t>TestTestTestTestTestTestTestgdgdfasd</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTest</t>
+          <t>TestTestTestTestTestTestTestdfgdfgasdasd</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTest</t>
+          <t>TestTestTestTestTestTestTestdfgdfasdas</t>
         </is>
       </c>
     </row>
@@ -2521,12 +2521,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>fsdfffffffffffffffff</t>
+          <t>fsdfffffffffffffffffdasdsafsdfffffffffffffffffasdasdfsdfffffffffffffffffasdasd</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>fsdfffffffffffffffff</t>
+          <t>fsdfffffffffffffffffasdasdfsdfffffffffffffffffasdasdfsdfffffffffffffffffasdasd</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add commit date: Thu Oct  3 17:47:36 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -1517,7 +1517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2515,21 +2515,6 @@
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>97</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>fsdfffffffffffffffffdasdsafsdfffffffffffffffffasdasdfsdfffffffffffffffffasdasd</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>fsdfffffffffffffffffasdasdfsdfffffffffffffffffasdasdfsdfffffffffffffffffasdasd</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Redisgn buttons and navbar
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,66 +621,6 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>Вывод всех записей таблицы</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1162</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1163</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTest</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTest</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTest</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1164</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTestadasd</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTestsadasd</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTestasdsad</t>
         </is>
       </c>
     </row>
@@ -695,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1196,66 +1136,6 @@
       <c r="D29" t="inlineStr">
         <is>
           <t>Метод загружает csv файл с данными.</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>2090</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение1</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>2091</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTest</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTest</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>TestTestTestTestTestTestTest</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>2092</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>пвавапавпавasdasd</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>павпвапавпвапasdasd</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>вапвввввввввasdad</t>
         </is>
       </c>
     </row>
@@ -1270,7 +1150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1280,231 +1160,211 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTestgdgdfasd</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTestdfgdfgasdasd</t>
+          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTestdfgdfasdas</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
+          <t>https://pypi.org/project/PyMySQL/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://pypi.org/project/PyMySQL/</t>
+          <t>https://getbootstrap.com/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Документация по Bootstrap.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://getbootstrap.com/</t>
+          <t>https://developer.mozilla.org/ru/docs/Web</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Сайт с документацией по веб-технологиям.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Работа с gitignore</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://developer.mozilla.org/ru/docs/Web</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
-        </is>
-      </c>
+          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Работа с gitignore</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
+          <t>https://sky.pro/media/pep8/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://sky.pro/media/pep8/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>https://ab57.ru/cmdlist.html</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://ab57.ru/cmdlist.html</t>
+          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Как создать и запустить bat-файлы</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Как сделать скрипт на bash</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Как сделать скрипт на bash</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add commit date: Tue Oct  8 17:57:34 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -1150,7 +1150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1160,211 +1160,231 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Логические типы в Python</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
+          <t>https://pythonchik.ru/osnovy/logicheskiy-tip-dannyh</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Логические типы в Python</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://pypi.org/project/PyMySQL/</t>
+          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://getbootstrap.com/</t>
+          <t>https://pypi.org/project/PyMySQL/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://developer.mozilla.org/ru/docs/Web</t>
+          <t>https://getbootstrap.com/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
+          <t>Документация по Bootstrap.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Работа с gitignore</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>https://developer.mozilla.org/ru/docs/Web</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Сайт с документацией по веб-технологиям.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Работа с gitignore</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://sky.pro/media/pep8/</t>
+          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>https://sky.pro/media/pep8/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://ab57.ru/cmdlist.html</t>
+          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>https://ab57.ru/cmdlist.html</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Как создать и запустить bat-файлы</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>1</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Как сделать скрипт на bash</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add local bootstrap codes
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -1150,7 +1150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1160,231 +1160,251 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Логические типы в Python</t>
+          <t>Описание SQLite</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>https://pythonchik.ru/osnovy/logicheskiy-tip-dannyh</t>
+          <t>https://metanit.com/sql/sqlite/</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Логические типы в Python</t>
+          <t>Описание SQLite</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Логические типы в Python</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
+          <t>https://pythonchik.ru/osnovy/logicheskiy-tip-dannyh</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Логические типы в Python</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://pypi.org/project/PyMySQL/</t>
+          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://getbootstrap.com/</t>
+          <t>https://pypi.org/project/PyMySQL/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://developer.mozilla.org/ru/docs/Web</t>
+          <t>https://getbootstrap.com/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
+          <t>Документация по Bootstrap.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Работа с gitignore</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>https://developer.mozilla.org/ru/docs/Web</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Сайт с документацией по веб-технологиям.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Работа с gitignore</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://sky.pro/media/pep8/</t>
+          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>https://sky.pro/media/pep8/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://ab57.ru/cmdlist.html</t>
+          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>https://ab57.ru/cmdlist.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Как создать и запустить bat-файлы</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>1</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Как сделать скрипт на bash</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add commit date: Wed Oct  9 17:44:56 RTZ 2024
</commit_message>
<xml_diff>
--- a/xlsx_export/output.xlsx
+++ b/xlsx_export/output.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,6 +621,27 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>Вывод всех записей таблицы</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1165</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ALTER TABLE tasks 
+DROP COLUMN task_status</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Удаление столбца таблицы</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Удаление столбца таблицы</t>
         </is>
       </c>
     </row>

</xml_diff>